<commit_message>
updated the drag and drop/click to work; added CSS styling to the upload files section
</commit_message>
<xml_diff>
--- a/sampleTimeCard.xlsx
+++ b/sampleTimeCard.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02b523206eeb39fd/Desktop/GitHub/jirehNotebook/testSite/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02b523206eeb39fd/Desktop/GitHub/testSite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{AC63B318-AC7D-4942-A15E-45CB693F4318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC7D0A20-D4A2-4442-AB31-61EABDF075CD}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AC63B318-AC7D-4942-A15E-45CB693F4318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36919036-A5B5-4F38-8063-2B65245D7898}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{CD6BC56B-3254-4E86-BE4C-7A1B02412E97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -446,14 +449,22 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -705,6 +716,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K10" xr:uid="{AC16B890-38F6-4ECB-960E-86CD3F879007}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>